<commit_message>
Spell checking final submission
Signed-off-by: Nasseryoyo <youussefnasser@gmail.com>
</commit_message>
<xml_diff>
--- a/TempleSE Software Requirements.xlsx
+++ b/TempleSE Software Requirements.xlsx
@@ -201,7 +201,7 @@
     <t>Donation Receiver</t>
   </si>
   <si>
-    <t>be able to sign up for an account  by entering proof  confriming that i am in need of  donations</t>
+    <t>be able to sign up for an account  by entering proof  confirming that i am in need of  donations</t>
   </si>
   <si>
     <t xml:space="preserve">I can create Donation requests and Receive the items I need </t>
@@ -214,7 +214,7 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>be able to sign up for an account  by entering organization type , and proof of organization credtionals</t>
+    <t>be able to sign up for an account  by entering organization type , and proof of organization credentials</t>
   </si>
   <si>
     <t>I can create Volunteer opportunities relevant to the services I offer for donors to participate in and create donation requests for items I need</t>
@@ -237,16 +237,16 @@
 type of transportation can be motorcycle , car or pickup truck</t>
   </si>
   <si>
-    <t>be able to sign up for special services if i am in eldery</t>
-  </si>
-  <si>
-    <t>i can receive help from admin if i am not comfortable using digitial channels</t>
+    <t>be able to sign up for special services if i am in elderly</t>
+  </si>
+  <si>
+    <t>i can receive help from admin if i am not comfortable using digital channels</t>
   </si>
   <si>
     <t>special services include having access to admin contact information</t>
   </si>
   <si>
-    <t>Donor/Donation receiver/Organization/Driver/Adminstrator</t>
+    <t>Donor/Donation receiver/Organization/Driver/Administrator</t>
   </si>
   <si>
     <t xml:space="preserve">login using my username and password </t>
@@ -522,7 +522,7 @@
     <t>I can easily choose which page I want to donate to/ participate in based on my interests and values</t>
   </si>
   <si>
-    <t>be able to view the list of donation requests / volunteer opportunites  with basic details for each donation request / volunteer opportunities</t>
+    <t>be able to view the list of donation requests / volunteer opportunities  with basic details for each donation request / volunteer opportunities</t>
   </si>
   <si>
     <t xml:space="preserve">I can become more informed on all the available donation requests / volunteer opportunities </t>
@@ -749,13 +749,13 @@
     <t>be able to receive emails and messages from Website / Application</t>
   </si>
   <si>
-    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidlines and receive mail when all the items in the donation request i donated too is completed so that i can create pickup and delivery request for donation and receive marketing messages</t>
+    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidelines and receive mail when all the items in the donation request i donated too is completed so that i can create pickup and delivery request for donation and receive marketing messages</t>
   </si>
   <si>
     <t>be able to receive system notifications and in app messages</t>
   </si>
   <si>
-    <t>i can receive notifications from groupchats i'm in</t>
+    <t>i can receive notifications from group chats i'm in</t>
   </si>
   <si>
     <t>Donation Receiver / Organization</t>
@@ -828,7 +828,7 @@
     <t>i can maximize the impact of each donation</t>
   </si>
   <si>
-    <t>be able to upload images and videos of the impact of the donation requests / volunteer opportunities to forms provied on Website / Application</t>
+    <t>be able to upload images and videos of the impact of the donation requests / volunteer opportunities to forms provided on Website / Application</t>
   </si>
   <si>
     <t>i can help encourage donors to continue their good work by helping them track their impact</t>
@@ -855,10 +855,10 @@
     <t xml:space="preserve"> i can arrange a suitable time for delivery</t>
   </si>
   <si>
-    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidlines and receive mail if donor has claimed donation request / Volunteer opportunity</t>
-  </si>
-  <si>
-    <t>i can be notfied with estimated delivery time when my requested items is picked up</t>
+    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidelines and receive mail if donor has claimed donation request / Volunteer opportunity</t>
+  </si>
+  <si>
+    <t>i can be notified with estimated delivery time when my requested items is picked up</t>
   </si>
   <si>
     <t>be able to search using a search bar through the list of  the Donation pickup and delivery tasks</t>
@@ -900,7 +900,7 @@
     <t xml:space="preserve">I can make a more informed decision about which pickup and delivery task to accept </t>
   </si>
   <si>
-    <t>full details include rating of donor / donation receviver / organization .buttons needed include buttons to claim and report</t>
+    <t>full details include rating of donor / donation receiver / organization .buttons needed include buttons to claim and report</t>
   </si>
   <si>
     <t>be able to claim a pickup and delivery request</t>
@@ -954,13 +954,13 @@
     <t xml:space="preserve">so that I can confirm the deliveries to donors </t>
   </si>
   <si>
-    <t>be able to update delivery status (such as, pickedup - on the way - delayed - delivered  etc.)</t>
+    <t>be able to update delivery status (such as, picked up - on the way - delayed - delivered  etc.)</t>
   </si>
   <si>
     <t>so that the donor can stay updated about the status of the delivery at all times</t>
   </si>
   <si>
-    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidlines and receive any changes that might happen to my task</t>
+    <t>i can be receive mail if my account is suspended or if someone tried to login into my account and to receive warnings if i violated guidelines and receive any changes that might happen to my task</t>
   </si>
   <si>
     <t>i can receive reminder notifications about my tasks and be notified about new tasks in my area</t>
@@ -1023,7 +1023,7 @@
     <t>be able to read responses to forms asking donation receiver to upload images / videos of their received donations</t>
   </si>
   <si>
-    <t>i can upload images / videos to "About Us" page to help encourge donors to continue thier good work</t>
+    <t>i can upload images / videos to "About Us" page to help encourage donors to continue their good work</t>
   </si>
   <si>
     <t>be able to edit and update "About Us' page</t>
@@ -1197,7 +1197,7 @@
     <t>be able to create a donation request on behalf of the donation receiver who called me</t>
   </si>
   <si>
-    <t>i can create it for them if they are not comfortable using digtial channels</t>
+    <t>i can create it for them if they are not comfortable using digital channels</t>
   </si>
   <si>
     <t>be able to create a volunteer opportunity for donors to pick up and deliver donations as organization's driver</t>

</xml_diff>